<commit_message>
ADD Controls |MODIFY ProjectilesUpgrade_Meta.xlsx
</commit_message>
<xml_diff>
--- a/Documents/GameDesign/ProjectilesUpgrade_Meta.xlsx
+++ b/Documents/GameDesign/ProjectilesUpgrade_Meta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\GameSup_GD1\Workshop\Tower_Defense\STD_Workshop\Documents\GameDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7F9480-2CD7-48F9-AFCF-13068F585BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0921949E-F235-48D9-8E88-F33F26FE1B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="4560" windowWidth="11355" windowHeight="7590" activeTab="1" xr2:uid="{F583284D-B83E-47B1-A299-B6E85F80DD06}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F583284D-B83E-47B1-A299-B6E85F80DD06}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseStats" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="53">
   <si>
     <t>Statistiques</t>
   </si>
@@ -127,9 +127,6 @@
     <t>Use basic effect</t>
   </si>
   <si>
-    <t>The chewing gum split in the air to aim 2 enemies at once</t>
-  </si>
-  <si>
     <t>Energy</t>
   </si>
   <si>
@@ -187,9 +184,6 @@
     <t>Apply medium damage to enemy</t>
   </si>
   <si>
-    <t>The chewing gum slow down enemies for a certain duration. Apply low damage to enemies</t>
-  </si>
-  <si>
     <t>Statistics</t>
   </si>
   <si>
@@ -200,6 +194,9 @@
   </si>
   <si>
     <t>The pizza explode at the impact</t>
+  </si>
+  <si>
+    <t>The chewing gum split in the air to aim 2 enemies at once, tehy are slow down.</t>
   </si>
 </sst>
 </file>
@@ -468,122 +465,122 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1034,10 +1031,10 @@
     </row>
     <row r="5" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>31</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>19</v>
@@ -1045,7 +1042,7 @@
     </row>
     <row r="6" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>8</v>
@@ -1073,7 +1070,7 @@
     </row>
     <row r="8" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>9</v>
@@ -1174,567 +1171,567 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="44.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" style="24" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="24"/>
-    <col min="5" max="5" width="22" style="24" customWidth="1"/>
-    <col min="6" max="6" width="46" style="25" customWidth="1"/>
-    <col min="7" max="9" width="14.140625" style="25" customWidth="1"/>
-    <col min="10" max="10" width="33.7109375" style="25" customWidth="1"/>
-    <col min="11" max="12" width="33.7109375" style="26" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="21"/>
+    <col min="1" max="1" width="20.42578125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="18"/>
+    <col min="5" max="5" width="22" style="18" customWidth="1"/>
+    <col min="6" max="6" width="46" style="19" customWidth="1"/>
+    <col min="7" max="9" width="14.140625" style="19" customWidth="1"/>
+    <col min="10" max="10" width="33.7109375" style="19" customWidth="1"/>
+    <col min="11" max="12" width="33.7109375" style="20" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="46"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="20" t="s">
+      <c r="G1" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="48"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
     </row>
     <row r="2" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="22" t="s">
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" s="22" t="s">
+      <c r="H2" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="L2" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="27" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="str">
+    <row r="3" spans="1:12" s="21" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="str">
         <f>_xlfn.CONCAT(B3,"_",LEFT(C3,3), "_",D3)</f>
         <v>1_Tra_1</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B3" s="22">
         <v>1</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="22">
         <v>1</v>
       </c>
-      <c r="E3" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="48" t="s">
+      <c r="E3" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="H3" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="48" t="s">
+      <c r="I3" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-    </row>
-    <row r="4" spans="1:12" s="30" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="str">
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+    </row>
+    <row r="4" spans="1:12" s="24" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="str">
         <f t="shared" ref="A4:A29" si="0">_xlfn.CONCAT(B4,"_",LEFT(C4,3), "_",D4)</f>
         <v>2_Tra_2a</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="25">
         <v>2</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+    </row>
+    <row r="5" spans="1:12" s="21" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="str">
+        <f t="shared" si="0"/>
+        <v>3_Tra_2b</v>
+      </c>
+      <c r="B5" s="22">
+        <v>3</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="49" t="s">
+      <c r="F5" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="49" t="s">
+      <c r="G5" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-    </row>
-    <row r="5" spans="1:12" s="27" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="str">
-        <f t="shared" si="0"/>
-        <v>3_Tra_2b</v>
-      </c>
-      <c r="B5" s="28">
-        <v>3</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="28" t="s">
+      <c r="I5" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+    </row>
+    <row r="6" spans="1:12" s="27" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>4_Ene_1</v>
+      </c>
+      <c r="B6" s="28">
+        <v>4</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="28">
+        <v>1</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+    </row>
+    <row r="7" spans="1:12" s="30" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="str">
+        <f t="shared" si="0"/>
+        <v>5_Ene_2a</v>
+      </c>
+      <c r="B7" s="31">
+        <v>5</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+    </row>
+    <row r="8" spans="1:12" s="27" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v>6_Ene_2b</v>
+      </c>
+      <c r="B8" s="28">
+        <v>6</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" s="48" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="48" t="s">
+      <c r="E8" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
-    </row>
-    <row r="6" spans="1:12" s="33" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="str">
-        <f t="shared" si="0"/>
-        <v>4_Ene_1</v>
-      </c>
-      <c r="B6" s="34">
-        <v>4</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="34">
+      <c r="I8" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+    </row>
+    <row r="9" spans="1:12" s="33" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>7_Piz_1</v>
+      </c>
+      <c r="B9" s="34">
+        <v>7</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="34">
         <v>1</v>
       </c>
-      <c r="E6" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="50" t="s">
+      <c r="E9" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="50" t="s">
+      <c r="H9" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="50" t="s">
+      <c r="I9" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-    </row>
-    <row r="7" spans="1:12" s="36" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v>5_Ene_2a</v>
-      </c>
-      <c r="B7" s="37">
-        <v>5</v>
-      </c>
-      <c r="C7" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="37" t="s">
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+    </row>
+    <row r="10" spans="1:12" s="36" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>8_Piz_2a</v>
+      </c>
+      <c r="B10" s="37">
+        <v>8</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="51" t="s">
+      <c r="E10" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="51" t="s">
+      <c r="I10" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-    </row>
-    <row r="8" spans="1:12" s="33" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="str">
-        <f t="shared" si="0"/>
-        <v>6_Ene_2b</v>
-      </c>
-      <c r="B8" s="34">
-        <v>6</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" s="50" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-    </row>
-    <row r="9" spans="1:12" s="39" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="str">
-        <f t="shared" si="0"/>
-        <v>7_Piz_1</v>
-      </c>
-      <c r="B9" s="40">
-        <v>7</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="40">
-        <v>1</v>
-      </c>
-      <c r="E9" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="52" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="52" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="52" t="s">
-        <v>10</v>
-      </c>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-    </row>
-    <row r="10" spans="1:12" s="42" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>8_Piz_2a</v>
-      </c>
-      <c r="B10" s="43">
-        <v>8</v>
-      </c>
-      <c r="C10" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" s="53" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="53" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-    </row>
-    <row r="11" spans="1:12" s="39" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="str">
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+    </row>
+    <row r="11" spans="1:12" s="33" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="33" t="str">
         <f>_xlfn.CONCAT(B11,"_",LEFT(C11,3), "_",D11)</f>
         <v>9_Piz_2b</v>
       </c>
-      <c r="B11" s="40">
+      <c r="B11" s="34">
         <v>9</v>
       </c>
-      <c r="C11" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="40" t="s">
+      <c r="C11" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="52" t="s">
+      <c r="E11" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="52" t="s">
-        <v>52</v>
-      </c>
-      <c r="I11" s="52" t="s">
+      <c r="H11" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="41"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="41"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
     </row>
     <row r="12" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="str">
+      <c r="A12" s="15" t="str">
         <f t="shared" si="0"/>
         <v>10__</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="18">
         <v>10</v>
       </c>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
     </row>
     <row r="13" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="str">
+      <c r="A13" s="15" t="str">
         <f>_xlfn.CONCAT(B13,"_",LEFT(C13,3), "_",D13)</f>
         <v>11__</v>
       </c>
-      <c r="B13" s="24">
+      <c r="B13" s="18">
         <v>11</v>
       </c>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
     </row>
     <row r="14" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="str">
+      <c r="A14" s="15" t="str">
         <f t="shared" si="0"/>
         <v>12__</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="18">
         <v>12</v>
       </c>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
     </row>
     <row r="15" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="str">
+      <c r="A15" s="15" t="str">
         <f t="shared" si="0"/>
         <v>13__</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="18">
         <v>13</v>
       </c>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
     </row>
     <row r="16" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="str">
+      <c r="A16" s="15" t="str">
         <f t="shared" si="0"/>
         <v>14__</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="18">
         <v>14</v>
       </c>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
     </row>
     <row r="17" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="str">
+      <c r="A17" s="15" t="str">
         <f t="shared" si="0"/>
         <v>15__</v>
       </c>
-      <c r="B17" s="24">
+      <c r="B17" s="18">
         <v>15</v>
       </c>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
     </row>
     <row r="18" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="str">
+      <c r="A18" s="15" t="str">
         <f t="shared" si="0"/>
         <v>16__</v>
       </c>
-      <c r="B18" s="24">
+      <c r="B18" s="18">
         <v>16</v>
       </c>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
     </row>
     <row r="19" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="str">
+      <c r="A19" s="15" t="str">
         <f t="shared" si="0"/>
         <v>17__</v>
       </c>
-      <c r="B19" s="24">
+      <c r="B19" s="18">
         <v>17</v>
       </c>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
     </row>
     <row r="20" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="str">
+      <c r="A20" s="15" t="str">
         <f t="shared" si="0"/>
         <v>18__</v>
       </c>
-      <c r="B20" s="24">
+      <c r="B20" s="18">
         <v>18</v>
       </c>
-      <c r="K20" s="25"/>
-      <c r="L20" s="25"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
     </row>
     <row r="21" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="str">
+      <c r="A21" s="15" t="str">
         <f t="shared" si="0"/>
         <v>19__</v>
       </c>
-      <c r="B21" s="24">
+      <c r="B21" s="18">
         <v>19</v>
       </c>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
     </row>
     <row r="22" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="str">
+      <c r="A22" s="15" t="str">
         <f t="shared" si="0"/>
         <v>20__</v>
       </c>
-      <c r="B22" s="24">
+      <c r="B22" s="18">
         <v>20</v>
       </c>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
     </row>
     <row r="23" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="str">
+      <c r="A23" s="15" t="str">
         <f t="shared" si="0"/>
         <v>21__</v>
       </c>
-      <c r="B23" s="24">
+      <c r="B23" s="18">
         <v>21</v>
       </c>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
     </row>
     <row r="24" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="str">
+      <c r="A24" s="15" t="str">
         <f t="shared" si="0"/>
         <v>22__</v>
       </c>
-      <c r="B24" s="24">
+      <c r="B24" s="18">
         <v>22</v>
       </c>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
     </row>
     <row r="25" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="str">
+      <c r="A25" s="15" t="str">
         <f t="shared" si="0"/>
         <v>23__</v>
       </c>
-      <c r="B25" s="24">
+      <c r="B25" s="18">
         <v>23</v>
       </c>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
     </row>
     <row r="26" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="str">
+      <c r="A26" s="15" t="str">
         <f t="shared" si="0"/>
         <v>24__</v>
       </c>
-      <c r="B26" s="24">
+      <c r="B26" s="18">
         <v>24</v>
       </c>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
     </row>
     <row r="27" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="str">
+      <c r="A27" s="15" t="str">
         <f t="shared" si="0"/>
         <v>25__</v>
       </c>
-      <c r="B27" s="24">
+      <c r="B27" s="18">
         <v>25</v>
       </c>
-      <c r="K27" s="25"/>
-      <c r="L27" s="25"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
     </row>
     <row r="28" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="21" t="str">
+      <c r="A28" s="15" t="str">
         <f t="shared" si="0"/>
         <v>26__</v>
       </c>
-      <c r="B28" s="24">
+      <c r="B28" s="18">
         <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="21" t="str">
+      <c r="A29" s="15" t="str">
         <f t="shared" si="0"/>
         <v>27__</v>
       </c>
-      <c r="B29" s="24">
+      <c r="B29" s="18">
         <v>27</v>
       </c>
     </row>
@@ -1775,33 +1772,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
     </row>
     <row r="2" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="18"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="53"/>
       <c r="F2" s="14" t="s">
         <v>21</v>
       </c>
@@ -1821,13 +1818,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>28</v>
@@ -1848,7 +1845,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>24</v>
@@ -1865,7 +1862,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>25</v>
@@ -1882,7 +1879,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -1896,7 +1893,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -1910,7 +1907,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -1924,7 +1921,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -1938,7 +1935,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -1952,7 +1949,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -1966,7 +1963,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -1980,7 +1977,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>

</xml_diff>